<commit_message>
added common section pattern
</commit_message>
<xml_diff>
--- a/new_values_seed_file.xlsx
+++ b/new_values_seed_file.xlsx
@@ -1,29 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\IdeaProjects\NewValueSeedFileGen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF0C8F7A-CB81-48EA-A882-CF0A0CE03705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="seed_request" sheetId="1" r:id="rId1"/>
+    <sheet name="seed_request" r:id="rId3" sheetId="1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">seed_request!$A$1:$N$1</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="409">
   <si>
     <t>{L=0}</t>
   </si>
@@ -1121,15 +1110,145 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>COMMON</t>
+  </si>
+  <si>
+    <t>COMMON_SECTIONS</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18555</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354027</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354023</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-20470</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-353824</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-20961</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-23866</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-19025</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18963</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18285</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-16664</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-22296</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18197</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-353750</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18435</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18437</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-21063</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-19463</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18420</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18376</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-22515</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354049</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-14894</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18533</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-17434</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-353980</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-19680</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354004</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-17655</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354020</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-354025</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-351285</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-24139</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18379</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-350424</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-24364</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18043</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-19392</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18917</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-18950</t>
+  </si>
+  <si>
+    <t>cnet_common_SP-17390</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1141,7 +1260,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
   <borders count="1">
@@ -1159,337 +1278,18 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1574,7 +1374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1615,7 +1415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1697,7 +1497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1738,7 +1538,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1779,7 +1579,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1820,7 +1620,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1861,7 +1661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1902,7 +1702,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1943,7 +1743,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1984,7 +1784,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -2025,7 +1825,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -2066,7 +1866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2107,7 +1907,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2148,7 +1948,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -2189,7 +1989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -2230,7 +2030,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -2271,7 +2071,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -2312,7 +2112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -2353,7 +2153,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -2394,7 +2194,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -2435,7 +2235,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -2476,7 +2276,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -2517,7 +2317,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -2558,7 +2358,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -2599,7 +2399,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -2640,7 +2440,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -2681,7 +2481,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -2722,7 +2522,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31">
       <c r="A31" t="s">
         <v>125</v>
       </c>
@@ -2763,7 +2563,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -2804,7 +2604,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -2845,7 +2645,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -2886,7 +2686,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -2927,7 +2727,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -2968,7 +2768,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -3009,7 +2809,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -3050,7 +2850,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -3091,7 +2891,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3132,7 +2932,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -3173,7 +2973,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -3214,7 +3014,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -3255,7 +3055,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -3296,7 +3096,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -3337,7 +3137,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -3378,7 +3178,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="A47" t="s">
         <v>192</v>
       </c>
@@ -3419,7 +3219,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -3460,7 +3260,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49">
       <c r="A49" t="s">
         <v>203</v>
       </c>
@@ -3501,7 +3301,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -3542,7 +3342,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51">
       <c r="A51" t="s">
         <v>213</v>
       </c>
@@ -3583,7 +3383,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52">
       <c r="A52" t="s">
         <v>220</v>
       </c>
@@ -3624,7 +3424,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53">
       <c r="A53" t="s">
         <v>220</v>
       </c>
@@ -3665,7 +3465,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54">
       <c r="A54" t="s">
         <v>232</v>
       </c>
@@ -3706,7 +3506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55">
       <c r="A55" t="s">
         <v>238</v>
       </c>
@@ -3747,7 +3547,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56">
       <c r="A56" t="s">
         <v>244</v>
       </c>
@@ -3788,7 +3588,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57">
       <c r="A57" t="s">
         <v>250</v>
       </c>
@@ -3829,7 +3629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -3870,7 +3670,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -3911,7 +3711,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -3952,7 +3752,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61">
       <c r="A61" t="s">
         <v>271</v>
       </c>
@@ -3993,7 +3793,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62">
       <c r="A62" t="s">
         <v>271</v>
       </c>
@@ -4034,7 +3834,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63">
       <c r="A63" t="s">
         <v>277</v>
       </c>
@@ -4075,7 +3875,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64">
       <c r="A64" t="s">
         <v>277</v>
       </c>
@@ -4116,7 +3916,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65">
       <c r="A65" t="s">
         <v>277</v>
       </c>
@@ -4157,7 +3957,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66">
       <c r="A66" t="s">
         <v>283</v>
       </c>
@@ -4198,7 +3998,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67">
       <c r="A67" t="s">
         <v>285</v>
       </c>
@@ -4239,7 +4039,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68">
       <c r="A68" t="s">
         <v>285</v>
       </c>
@@ -4280,7 +4080,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69">
       <c r="A69" t="s">
         <v>293</v>
       </c>
@@ -4321,7 +4121,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70">
       <c r="A70" t="s">
         <v>293</v>
       </c>
@@ -4362,7 +4162,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71">
       <c r="A71" t="s">
         <v>295</v>
       </c>
@@ -4403,7 +4203,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72">
       <c r="A72" t="s">
         <v>295</v>
       </c>
@@ -4444,7 +4244,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73">
       <c r="A73" t="s">
         <v>297</v>
       </c>
@@ -4485,7 +4285,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74">
       <c r="A74" t="s">
         <v>305</v>
       </c>
@@ -4526,7 +4326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75">
       <c r="A75" t="s">
         <v>307</v>
       </c>
@@ -4567,7 +4367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76">
       <c r="A76" t="s">
         <v>309</v>
       </c>
@@ -4608,7 +4408,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77">
       <c r="A77" t="s">
         <v>311</v>
       </c>
@@ -4649,7 +4449,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78">
       <c r="A78" t="s">
         <v>313</v>
       </c>
@@ -4690,7 +4490,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79">
       <c r="A79" t="s">
         <v>319</v>
       </c>
@@ -4731,7 +4531,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80">
       <c r="A80" t="s">
         <v>326</v>
       </c>
@@ -4772,7 +4572,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81">
       <c r="A81" t="s">
         <v>328</v>
       </c>
@@ -4813,7 +4613,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82">
       <c r="A82" t="s">
         <v>330</v>
       </c>
@@ -4854,7 +4654,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83">
       <c r="A83" t="s">
         <v>332</v>
       </c>
@@ -4895,7 +4695,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84">
       <c r="A84" t="s">
         <v>338</v>
       </c>
@@ -4936,7 +4736,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85">
       <c r="A85" t="s">
         <v>340</v>
       </c>
@@ -4977,7 +4777,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86">
       <c r="A86" t="s">
         <v>342</v>
       </c>
@@ -5018,7 +4818,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87">
       <c r="A87" t="s">
         <v>342</v>
       </c>
@@ -5059,7 +4859,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88">
       <c r="A88" t="s">
         <v>353</v>
       </c>
@@ -5100,7 +4900,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89">
       <c r="A89" t="s">
         <v>355</v>
       </c>
@@ -5141,7 +4941,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90">
       <c r="A90" t="s">
         <v>357</v>
       </c>
@@ -5182,7 +4982,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91">
       <c r="A91" t="s">
         <v>359</v>
       </c>
@@ -5223,8 +5023,1688 @@
         <v>365</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>366</v>
+      </c>
+      <c r="B92" t="s">
+        <v>367</v>
+      </c>
+      <c r="C92" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" t="s">
+        <v>42</v>
+      </c>
+      <c r="G92" t="s">
+        <v>20</v>
+      </c>
+      <c r="H92" t="s">
+        <v>368</v>
+      </c>
+      <c r="I92" t="s">
+        <v>22</v>
+      </c>
+      <c r="J92" t="s">
+        <v>23</v>
+      </c>
+      <c r="K92" t="s">
+        <v>24</v>
+      </c>
+      <c r="L92" t="s">
+        <v>13</v>
+      </c>
+      <c r="M92" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>366</v>
+      </c>
+      <c r="B93" t="s">
+        <v>367</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" t="s">
+        <v>42</v>
+      </c>
+      <c r="G93" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" t="s">
+        <v>369</v>
+      </c>
+      <c r="I93" t="s">
+        <v>22</v>
+      </c>
+      <c r="J93" t="s">
+        <v>23</v>
+      </c>
+      <c r="K93" t="s">
+        <v>35</v>
+      </c>
+      <c r="L93" t="s">
+        <v>36</v>
+      </c>
+      <c r="M93" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>366</v>
+      </c>
+      <c r="B94" t="s">
+        <v>367</v>
+      </c>
+      <c r="C94" t="s">
+        <v>40</v>
+      </c>
+      <c r="D94" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" t="s">
+        <v>42</v>
+      </c>
+      <c r="G94" t="s">
+        <v>20</v>
+      </c>
+      <c r="H94" t="s">
+        <v>370</v>
+      </c>
+      <c r="I94" t="s">
+        <v>22</v>
+      </c>
+      <c r="J94" t="s">
+        <v>23</v>
+      </c>
+      <c r="K94" t="s">
+        <v>44</v>
+      </c>
+      <c r="L94" t="s">
+        <v>45</v>
+      </c>
+      <c r="M94" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>366</v>
+      </c>
+      <c r="B95" t="s">
+        <v>367</v>
+      </c>
+      <c r="C95" t="s">
+        <v>55</v>
+      </c>
+      <c r="D95" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" t="s">
+        <v>42</v>
+      </c>
+      <c r="G95" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" t="s">
+        <v>371</v>
+      </c>
+      <c r="I95" t="s">
+        <v>22</v>
+      </c>
+      <c r="J95" t="s">
+        <v>23</v>
+      </c>
+      <c r="K95" t="s">
+        <v>58</v>
+      </c>
+      <c r="L95" t="s">
+        <v>13</v>
+      </c>
+      <c r="M95" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>366</v>
+      </c>
+      <c r="B96" t="s">
+        <v>367</v>
+      </c>
+      <c r="C96" t="s">
+        <v>62</v>
+      </c>
+      <c r="D96" t="s">
+        <v>13</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" t="s">
+        <v>42</v>
+      </c>
+      <c r="G96" t="s">
+        <v>20</v>
+      </c>
+      <c r="H96" t="s">
+        <v>372</v>
+      </c>
+      <c r="I96" t="s">
+        <v>22</v>
+      </c>
+      <c r="J96" t="s">
+        <v>23</v>
+      </c>
+      <c r="K96" t="s">
+        <v>65</v>
+      </c>
+      <c r="L96" t="s">
+        <v>13</v>
+      </c>
+      <c r="M96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>366</v>
+      </c>
+      <c r="B97" t="s">
+        <v>367</v>
+      </c>
+      <c r="C97" t="s">
+        <v>69</v>
+      </c>
+      <c r="D97" t="s">
+        <v>13</v>
+      </c>
+      <c r="E97" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" t="s">
+        <v>42</v>
+      </c>
+      <c r="G97" t="s">
+        <v>20</v>
+      </c>
+      <c r="H97" t="s">
+        <v>373</v>
+      </c>
+      <c r="I97" t="s">
+        <v>22</v>
+      </c>
+      <c r="J97" t="s">
+        <v>23</v>
+      </c>
+      <c r="K97" t="s">
+        <v>72</v>
+      </c>
+      <c r="L97" t="s">
+        <v>13</v>
+      </c>
+      <c r="M97" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>366</v>
+      </c>
+      <c r="B98" t="s">
+        <v>367</v>
+      </c>
+      <c r="C98" t="s">
+        <v>76</v>
+      </c>
+      <c r="D98" t="s">
+        <v>13</v>
+      </c>
+      <c r="E98" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" t="s">
+        <v>42</v>
+      </c>
+      <c r="G98" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98" t="s">
+        <v>374</v>
+      </c>
+      <c r="I98" t="s">
+        <v>22</v>
+      </c>
+      <c r="J98" t="s">
+        <v>23</v>
+      </c>
+      <c r="K98" t="s">
+        <v>79</v>
+      </c>
+      <c r="L98" t="s">
+        <v>80</v>
+      </c>
+      <c r="M98" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>366</v>
+      </c>
+      <c r="B99" t="s">
+        <v>367</v>
+      </c>
+      <c r="C99" t="s">
+        <v>92</v>
+      </c>
+      <c r="D99" t="s">
+        <v>13</v>
+      </c>
+      <c r="E99" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" t="s">
+        <v>42</v>
+      </c>
+      <c r="G99" t="s">
+        <v>20</v>
+      </c>
+      <c r="H99" t="s">
+        <v>375</v>
+      </c>
+      <c r="I99" t="s">
+        <v>22</v>
+      </c>
+      <c r="J99" t="s">
+        <v>23</v>
+      </c>
+      <c r="K99" t="s">
+        <v>95</v>
+      </c>
+      <c r="L99" t="s">
+        <v>13</v>
+      </c>
+      <c r="M99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>366</v>
+      </c>
+      <c r="B100" t="s">
+        <v>367</v>
+      </c>
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" t="s">
+        <v>42</v>
+      </c>
+      <c r="G100" t="s">
+        <v>20</v>
+      </c>
+      <c r="H100" t="s">
+        <v>376</v>
+      </c>
+      <c r="I100" t="s">
+        <v>22</v>
+      </c>
+      <c r="J100" t="s">
+        <v>23</v>
+      </c>
+      <c r="K100" t="s">
+        <v>110</v>
+      </c>
+      <c r="L100" t="s">
+        <v>111</v>
+      </c>
+      <c r="M100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>366</v>
+      </c>
+      <c r="B101" t="s">
+        <v>367</v>
+      </c>
+      <c r="C101" t="s">
+        <v>133</v>
+      </c>
+      <c r="D101" t="s">
+        <v>13</v>
+      </c>
+      <c r="E101" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" t="s">
+        <v>42</v>
+      </c>
+      <c r="G101" t="s">
+        <v>20</v>
+      </c>
+      <c r="H101" t="s">
+        <v>377</v>
+      </c>
+      <c r="I101" t="s">
+        <v>22</v>
+      </c>
+      <c r="J101" t="s">
+        <v>23</v>
+      </c>
+      <c r="K101" t="s">
+        <v>136</v>
+      </c>
+      <c r="L101" t="s">
+        <v>13</v>
+      </c>
+      <c r="M101" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>366</v>
+      </c>
+      <c r="B102" t="s">
+        <v>367</v>
+      </c>
+      <c r="C102" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" t="s">
+        <v>42</v>
+      </c>
+      <c r="G102" t="s">
+        <v>20</v>
+      </c>
+      <c r="H102" t="s">
+        <v>378</v>
+      </c>
+      <c r="I102" t="s">
+        <v>22</v>
+      </c>
+      <c r="J102" t="s">
+        <v>23</v>
+      </c>
+      <c r="K102" t="s">
+        <v>145</v>
+      </c>
+      <c r="L102" t="s">
+        <v>13</v>
+      </c>
+      <c r="M102" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>366</v>
+      </c>
+      <c r="B103" t="s">
+        <v>367</v>
+      </c>
+      <c r="C103" t="s">
+        <v>148</v>
+      </c>
+      <c r="D103" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" t="s">
+        <v>42</v>
+      </c>
+      <c r="G103" t="s">
+        <v>20</v>
+      </c>
+      <c r="H103" t="s">
+        <v>379</v>
+      </c>
+      <c r="I103" t="s">
+        <v>22</v>
+      </c>
+      <c r="J103" t="s">
+        <v>23</v>
+      </c>
+      <c r="K103" t="s">
+        <v>151</v>
+      </c>
+      <c r="L103" t="s">
+        <v>13</v>
+      </c>
+      <c r="M103" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>366</v>
+      </c>
+      <c r="B104" t="s">
+        <v>367</v>
+      </c>
+      <c r="C104" t="s">
+        <v>155</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" t="s">
+        <v>42</v>
+      </c>
+      <c r="G104" t="s">
+        <v>20</v>
+      </c>
+      <c r="H104" t="s">
+        <v>380</v>
+      </c>
+      <c r="I104" t="s">
+        <v>22</v>
+      </c>
+      <c r="J104" t="s">
+        <v>23</v>
+      </c>
+      <c r="K104" t="s">
+        <v>158</v>
+      </c>
+      <c r="L104" t="s">
+        <v>13</v>
+      </c>
+      <c r="M104" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>366</v>
+      </c>
+      <c r="B105" t="s">
+        <v>367</v>
+      </c>
+      <c r="C105" t="s">
+        <v>162</v>
+      </c>
+      <c r="D105" t="s">
+        <v>13</v>
+      </c>
+      <c r="E105" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" t="s">
+        <v>42</v>
+      </c>
+      <c r="G105" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" t="s">
+        <v>381</v>
+      </c>
+      <c r="I105" t="s">
+        <v>22</v>
+      </c>
+      <c r="J105" t="s">
+        <v>23</v>
+      </c>
+      <c r="K105" t="s">
+        <v>165</v>
+      </c>
+      <c r="L105" t="s">
+        <v>13</v>
+      </c>
+      <c r="M105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>366</v>
+      </c>
+      <c r="B106" t="s">
+        <v>367</v>
+      </c>
+      <c r="C106" t="s">
+        <v>168</v>
+      </c>
+      <c r="D106" t="s">
+        <v>13</v>
+      </c>
+      <c r="E106" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" t="s">
+        <v>42</v>
+      </c>
+      <c r="G106" t="s">
+        <v>20</v>
+      </c>
+      <c r="H106" t="s">
+        <v>382</v>
+      </c>
+      <c r="I106" t="s">
+        <v>22</v>
+      </c>
+      <c r="J106" t="s">
+        <v>23</v>
+      </c>
+      <c r="K106" t="s">
+        <v>171</v>
+      </c>
+      <c r="L106" t="s">
+        <v>13</v>
+      </c>
+      <c r="M106" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>366</v>
+      </c>
+      <c r="B107" t="s">
+        <v>367</v>
+      </c>
+      <c r="C107" t="s">
+        <v>173</v>
+      </c>
+      <c r="D107" t="s">
+        <v>13</v>
+      </c>
+      <c r="E107" t="s">
+        <v>13</v>
+      </c>
+      <c r="F107" t="s">
+        <v>42</v>
+      </c>
+      <c r="G107" t="s">
+        <v>20</v>
+      </c>
+      <c r="H107" t="s">
+        <v>383</v>
+      </c>
+      <c r="I107" t="s">
+        <v>22</v>
+      </c>
+      <c r="J107" t="s">
+        <v>23</v>
+      </c>
+      <c r="K107" t="s">
+        <v>176</v>
+      </c>
+      <c r="L107" t="s">
+        <v>177</v>
+      </c>
+      <c r="M107" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>366</v>
+      </c>
+      <c r="B108" t="s">
+        <v>367</v>
+      </c>
+      <c r="C108" t="s">
+        <v>187</v>
+      </c>
+      <c r="D108" t="s">
+        <v>13</v>
+      </c>
+      <c r="E108" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" t="s">
+        <v>42</v>
+      </c>
+      <c r="G108" t="s">
+        <v>20</v>
+      </c>
+      <c r="H108" t="s">
+        <v>384</v>
+      </c>
+      <c r="I108" t="s">
+        <v>22</v>
+      </c>
+      <c r="J108" t="s">
+        <v>23</v>
+      </c>
+      <c r="K108" t="s">
+        <v>190</v>
+      </c>
+      <c r="L108" t="s">
+        <v>13</v>
+      </c>
+      <c r="M108" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>366</v>
+      </c>
+      <c r="B109" t="s">
+        <v>367</v>
+      </c>
+      <c r="C109" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" t="s">
+        <v>42</v>
+      </c>
+      <c r="G109" t="s">
+        <v>20</v>
+      </c>
+      <c r="H109" t="s">
+        <v>385</v>
+      </c>
+      <c r="I109" t="s">
+        <v>22</v>
+      </c>
+      <c r="J109" t="s">
+        <v>23</v>
+      </c>
+      <c r="K109" t="s">
+        <v>197</v>
+      </c>
+      <c r="L109" t="s">
+        <v>13</v>
+      </c>
+      <c r="M109" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>366</v>
+      </c>
+      <c r="B110" t="s">
+        <v>367</v>
+      </c>
+      <c r="C110" t="s">
+        <v>199</v>
+      </c>
+      <c r="D110" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" t="s">
+        <v>42</v>
+      </c>
+      <c r="G110" t="s">
+        <v>20</v>
+      </c>
+      <c r="H110" t="s">
+        <v>386</v>
+      </c>
+      <c r="I110" t="s">
+        <v>22</v>
+      </c>
+      <c r="J110" t="s">
+        <v>23</v>
+      </c>
+      <c r="K110" t="s">
+        <v>202</v>
+      </c>
+      <c r="L110" t="s">
+        <v>13</v>
+      </c>
+      <c r="M110" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>366</v>
+      </c>
+      <c r="B111" t="s">
+        <v>367</v>
+      </c>
+      <c r="C111" t="s">
+        <v>205</v>
+      </c>
+      <c r="D111" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" t="s">
+        <v>42</v>
+      </c>
+      <c r="G111" t="s">
+        <v>20</v>
+      </c>
+      <c r="H111" t="s">
+        <v>387</v>
+      </c>
+      <c r="I111" t="s">
+        <v>22</v>
+      </c>
+      <c r="J111" t="s">
+        <v>23</v>
+      </c>
+      <c r="K111" t="s">
+        <v>208</v>
+      </c>
+      <c r="L111" t="s">
+        <v>13</v>
+      </c>
+      <c r="M111" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>366</v>
+      </c>
+      <c r="B112" t="s">
+        <v>367</v>
+      </c>
+      <c r="C112" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" t="s">
+        <v>13</v>
+      </c>
+      <c r="E112" t="s">
+        <v>13</v>
+      </c>
+      <c r="F112" t="s">
+        <v>42</v>
+      </c>
+      <c r="G112" t="s">
+        <v>20</v>
+      </c>
+      <c r="H112" t="s">
+        <v>388</v>
+      </c>
+      <c r="I112" t="s">
+        <v>22</v>
+      </c>
+      <c r="J112" t="s">
+        <v>23</v>
+      </c>
+      <c r="K112" t="s">
+        <v>212</v>
+      </c>
+      <c r="L112" t="s">
+        <v>13</v>
+      </c>
+      <c r="M112" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>366</v>
+      </c>
+      <c r="B113" t="s">
+        <v>367</v>
+      </c>
+      <c r="C113" t="s">
+        <v>215</v>
+      </c>
+      <c r="D113" t="s">
+        <v>13</v>
+      </c>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+      <c r="F113" t="s">
+        <v>42</v>
+      </c>
+      <c r="G113" t="s">
+        <v>20</v>
+      </c>
+      <c r="H113" t="s">
+        <v>389</v>
+      </c>
+      <c r="I113" t="s">
+        <v>22</v>
+      </c>
+      <c r="J113" t="s">
+        <v>23</v>
+      </c>
+      <c r="K113" t="s">
+        <v>218</v>
+      </c>
+      <c r="L113" t="s">
+        <v>13</v>
+      </c>
+      <c r="M113" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>366</v>
+      </c>
+      <c r="B114" t="s">
+        <v>367</v>
+      </c>
+      <c r="C114" t="s">
+        <v>222</v>
+      </c>
+      <c r="D114" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" t="s">
+        <v>42</v>
+      </c>
+      <c r="G114" t="s">
+        <v>20</v>
+      </c>
+      <c r="H114" t="s">
+        <v>390</v>
+      </c>
+      <c r="I114" t="s">
+        <v>22</v>
+      </c>
+      <c r="J114" t="s">
+        <v>23</v>
+      </c>
+      <c r="K114" t="s">
+        <v>225</v>
+      </c>
+      <c r="L114" t="s">
+        <v>13</v>
+      </c>
+      <c r="M114" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>366</v>
+      </c>
+      <c r="B115" t="s">
+        <v>367</v>
+      </c>
+      <c r="C115" t="s">
+        <v>227</v>
+      </c>
+      <c r="D115" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" t="s">
+        <v>13</v>
+      </c>
+      <c r="F115" t="s">
+        <v>42</v>
+      </c>
+      <c r="G115" t="s">
+        <v>20</v>
+      </c>
+      <c r="H115" t="s">
+        <v>391</v>
+      </c>
+      <c r="I115" t="s">
+        <v>22</v>
+      </c>
+      <c r="J115" t="s">
+        <v>23</v>
+      </c>
+      <c r="K115" t="s">
+        <v>230</v>
+      </c>
+      <c r="L115" t="s">
+        <v>13</v>
+      </c>
+      <c r="M115" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>366</v>
+      </c>
+      <c r="B116" t="s">
+        <v>367</v>
+      </c>
+      <c r="C116" t="s">
+        <v>234</v>
+      </c>
+      <c r="D116" t="s">
+        <v>13</v>
+      </c>
+      <c r="E116" t="s">
+        <v>13</v>
+      </c>
+      <c r="F116" t="s">
+        <v>42</v>
+      </c>
+      <c r="G116" t="s">
+        <v>20</v>
+      </c>
+      <c r="H116" t="s">
+        <v>392</v>
+      </c>
+      <c r="I116" t="s">
+        <v>22</v>
+      </c>
+      <c r="J116" t="s">
+        <v>23</v>
+      </c>
+      <c r="K116" t="s">
+        <v>237</v>
+      </c>
+      <c r="L116" t="s">
+        <v>13</v>
+      </c>
+      <c r="M116" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>366</v>
+      </c>
+      <c r="B117" t="s">
+        <v>367</v>
+      </c>
+      <c r="C117" t="s">
+        <v>240</v>
+      </c>
+      <c r="D117" t="s">
+        <v>13</v>
+      </c>
+      <c r="E117" t="s">
+        <v>13</v>
+      </c>
+      <c r="F117" t="s">
+        <v>42</v>
+      </c>
+      <c r="G117" t="s">
+        <v>20</v>
+      </c>
+      <c r="H117" t="s">
+        <v>393</v>
+      </c>
+      <c r="I117" t="s">
+        <v>22</v>
+      </c>
+      <c r="J117" t="s">
+        <v>23</v>
+      </c>
+      <c r="K117" t="s">
+        <v>243</v>
+      </c>
+      <c r="L117" t="s">
+        <v>13</v>
+      </c>
+      <c r="M117" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>366</v>
+      </c>
+      <c r="B118" t="s">
+        <v>367</v>
+      </c>
+      <c r="C118" t="s">
+        <v>246</v>
+      </c>
+      <c r="D118" t="s">
+        <v>13</v>
+      </c>
+      <c r="E118" t="s">
+        <v>13</v>
+      </c>
+      <c r="F118" t="s">
+        <v>42</v>
+      </c>
+      <c r="G118" t="s">
+        <v>20</v>
+      </c>
+      <c r="H118" t="s">
+        <v>394</v>
+      </c>
+      <c r="I118" t="s">
+        <v>22</v>
+      </c>
+      <c r="J118" t="s">
+        <v>23</v>
+      </c>
+      <c r="K118" t="s">
+        <v>249</v>
+      </c>
+      <c r="L118" t="s">
+        <v>13</v>
+      </c>
+      <c r="M118" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>366</v>
+      </c>
+      <c r="B119" t="s">
+        <v>367</v>
+      </c>
+      <c r="C119" t="s">
+        <v>252</v>
+      </c>
+      <c r="D119" t="s">
+        <v>13</v>
+      </c>
+      <c r="E119" t="s">
+        <v>13</v>
+      </c>
+      <c r="F119" t="s">
+        <v>42</v>
+      </c>
+      <c r="G119" t="s">
+        <v>20</v>
+      </c>
+      <c r="H119" t="s">
+        <v>395</v>
+      </c>
+      <c r="I119" t="s">
+        <v>22</v>
+      </c>
+      <c r="J119" t="s">
+        <v>23</v>
+      </c>
+      <c r="K119" t="s">
+        <v>252</v>
+      </c>
+      <c r="L119" t="s">
+        <v>13</v>
+      </c>
+      <c r="M119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>366</v>
+      </c>
+      <c r="B120" t="s">
+        <v>367</v>
+      </c>
+      <c r="C120" t="s">
+        <v>255</v>
+      </c>
+      <c r="D120" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" t="s">
+        <v>13</v>
+      </c>
+      <c r="F120" t="s">
+        <v>42</v>
+      </c>
+      <c r="G120" t="s">
+        <v>20</v>
+      </c>
+      <c r="H120" t="s">
+        <v>396</v>
+      </c>
+      <c r="I120" t="s">
+        <v>22</v>
+      </c>
+      <c r="J120" t="s">
+        <v>23</v>
+      </c>
+      <c r="K120" t="s">
+        <v>258</v>
+      </c>
+      <c r="L120" t="s">
+        <v>13</v>
+      </c>
+      <c r="M120" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>366</v>
+      </c>
+      <c r="B121" t="s">
+        <v>367</v>
+      </c>
+      <c r="C121" t="s">
+        <v>261</v>
+      </c>
+      <c r="D121" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" t="s">
+        <v>13</v>
+      </c>
+      <c r="F121" t="s">
+        <v>42</v>
+      </c>
+      <c r="G121" t="s">
+        <v>20</v>
+      </c>
+      <c r="H121" t="s">
+        <v>397</v>
+      </c>
+      <c r="I121" t="s">
+        <v>22</v>
+      </c>
+      <c r="J121" t="s">
+        <v>23</v>
+      </c>
+      <c r="K121" t="s">
+        <v>264</v>
+      </c>
+      <c r="L121" t="s">
+        <v>13</v>
+      </c>
+      <c r="M121" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>366</v>
+      </c>
+      <c r="B122" t="s">
+        <v>367</v>
+      </c>
+      <c r="C122" t="s">
+        <v>267</v>
+      </c>
+      <c r="D122" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" t="s">
+        <v>13</v>
+      </c>
+      <c r="F122" t="s">
+        <v>42</v>
+      </c>
+      <c r="G122" t="s">
+        <v>20</v>
+      </c>
+      <c r="H122" t="s">
+        <v>398</v>
+      </c>
+      <c r="I122" t="s">
+        <v>22</v>
+      </c>
+      <c r="J122" t="s">
+        <v>23</v>
+      </c>
+      <c r="K122" t="s">
+        <v>270</v>
+      </c>
+      <c r="L122" t="s">
+        <v>13</v>
+      </c>
+      <c r="M122" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>366</v>
+      </c>
+      <c r="B123" t="s">
+        <v>367</v>
+      </c>
+      <c r="C123" t="s">
+        <v>273</v>
+      </c>
+      <c r="D123" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" t="s">
+        <v>13</v>
+      </c>
+      <c r="F123" t="s">
+        <v>42</v>
+      </c>
+      <c r="G123" t="s">
+        <v>20</v>
+      </c>
+      <c r="H123" t="s">
+        <v>399</v>
+      </c>
+      <c r="I123" t="s">
+        <v>22</v>
+      </c>
+      <c r="J123" t="s">
+        <v>23</v>
+      </c>
+      <c r="K123" t="s">
+        <v>276</v>
+      </c>
+      <c r="L123" t="s">
+        <v>13</v>
+      </c>
+      <c r="M123" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>366</v>
+      </c>
+      <c r="B124" t="s">
+        <v>367</v>
+      </c>
+      <c r="C124" t="s">
+        <v>279</v>
+      </c>
+      <c r="D124" t="s">
+        <v>13</v>
+      </c>
+      <c r="E124" t="s">
+        <v>13</v>
+      </c>
+      <c r="F124" t="s">
+        <v>42</v>
+      </c>
+      <c r="G124" t="s">
+        <v>20</v>
+      </c>
+      <c r="H124" t="s">
+        <v>400</v>
+      </c>
+      <c r="I124" t="s">
+        <v>22</v>
+      </c>
+      <c r="J124" t="s">
+        <v>23</v>
+      </c>
+      <c r="K124" t="s">
+        <v>282</v>
+      </c>
+      <c r="L124" t="s">
+        <v>13</v>
+      </c>
+      <c r="M124" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>366</v>
+      </c>
+      <c r="B125" t="s">
+        <v>367</v>
+      </c>
+      <c r="C125" t="s">
+        <v>287</v>
+      </c>
+      <c r="D125" t="s">
+        <v>13</v>
+      </c>
+      <c r="E125" t="s">
+        <v>13</v>
+      </c>
+      <c r="F125" t="s">
+        <v>42</v>
+      </c>
+      <c r="G125" t="s">
+        <v>20</v>
+      </c>
+      <c r="H125" t="s">
+        <v>401</v>
+      </c>
+      <c r="I125" t="s">
+        <v>22</v>
+      </c>
+      <c r="J125" t="s">
+        <v>23</v>
+      </c>
+      <c r="K125" t="s">
+        <v>290</v>
+      </c>
+      <c r="L125" t="s">
+        <v>291</v>
+      </c>
+      <c r="M125" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>366</v>
+      </c>
+      <c r="B126" t="s">
+        <v>367</v>
+      </c>
+      <c r="C126" t="s">
+        <v>299</v>
+      </c>
+      <c r="D126" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" t="s">
+        <v>13</v>
+      </c>
+      <c r="F126" t="s">
+        <v>42</v>
+      </c>
+      <c r="G126" t="s">
+        <v>20</v>
+      </c>
+      <c r="H126" t="s">
+        <v>402</v>
+      </c>
+      <c r="I126" t="s">
+        <v>22</v>
+      </c>
+      <c r="J126" t="s">
+        <v>23</v>
+      </c>
+      <c r="K126" t="s">
+        <v>302</v>
+      </c>
+      <c r="L126" t="s">
+        <v>303</v>
+      </c>
+      <c r="M126" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>366</v>
+      </c>
+      <c r="B127" t="s">
+        <v>367</v>
+      </c>
+      <c r="C127" t="s">
+        <v>315</v>
+      </c>
+      <c r="D127" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" t="s">
+        <v>13</v>
+      </c>
+      <c r="F127" t="s">
+        <v>42</v>
+      </c>
+      <c r="G127" t="s">
+        <v>20</v>
+      </c>
+      <c r="H127" t="s">
+        <v>403</v>
+      </c>
+      <c r="I127" t="s">
+        <v>22</v>
+      </c>
+      <c r="J127" t="s">
+        <v>23</v>
+      </c>
+      <c r="K127" t="s">
+        <v>318</v>
+      </c>
+      <c r="L127" t="s">
+        <v>13</v>
+      </c>
+      <c r="M127" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>366</v>
+      </c>
+      <c r="B128" t="s">
+        <v>367</v>
+      </c>
+      <c r="C128" t="s">
+        <v>321</v>
+      </c>
+      <c r="D128" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128" t="s">
+        <v>13</v>
+      </c>
+      <c r="F128" t="s">
+        <v>42</v>
+      </c>
+      <c r="G128" t="s">
+        <v>20</v>
+      </c>
+      <c r="H128" t="s">
+        <v>404</v>
+      </c>
+      <c r="I128" t="s">
+        <v>22</v>
+      </c>
+      <c r="J128" t="s">
+        <v>23</v>
+      </c>
+      <c r="K128" t="s">
+        <v>324</v>
+      </c>
+      <c r="L128" t="s">
+        <v>13</v>
+      </c>
+      <c r="M128" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>366</v>
+      </c>
+      <c r="B129" t="s">
+        <v>367</v>
+      </c>
+      <c r="C129" t="s">
+        <v>334</v>
+      </c>
+      <c r="D129" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" t="s">
+        <v>42</v>
+      </c>
+      <c r="G129" t="s">
+        <v>20</v>
+      </c>
+      <c r="H129" t="s">
+        <v>405</v>
+      </c>
+      <c r="I129" t="s">
+        <v>22</v>
+      </c>
+      <c r="J129" t="s">
+        <v>23</v>
+      </c>
+      <c r="K129" t="s">
+        <v>337</v>
+      </c>
+      <c r="L129" t="s">
+        <v>13</v>
+      </c>
+      <c r="M129" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>366</v>
+      </c>
+      <c r="B130" t="s">
+        <v>367</v>
+      </c>
+      <c r="C130" t="s">
+        <v>344</v>
+      </c>
+      <c r="D130" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" t="s">
+        <v>42</v>
+      </c>
+      <c r="G130" t="s">
+        <v>20</v>
+      </c>
+      <c r="H130" t="s">
+        <v>406</v>
+      </c>
+      <c r="I130" t="s">
+        <v>22</v>
+      </c>
+      <c r="J130" t="s">
+        <v>23</v>
+      </c>
+      <c r="K130" t="s">
+        <v>347</v>
+      </c>
+      <c r="L130" t="s">
+        <v>13</v>
+      </c>
+      <c r="M130" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>366</v>
+      </c>
+      <c r="B131" t="s">
+        <v>367</v>
+      </c>
+      <c r="C131" t="s">
+        <v>349</v>
+      </c>
+      <c r="D131" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" t="s">
+        <v>13</v>
+      </c>
+      <c r="F131" t="s">
+        <v>42</v>
+      </c>
+      <c r="G131" t="s">
+        <v>20</v>
+      </c>
+      <c r="H131" t="s">
+        <v>407</v>
+      </c>
+      <c r="I131" t="s">
+        <v>22</v>
+      </c>
+      <c r="J131" t="s">
+        <v>23</v>
+      </c>
+      <c r="K131" t="s">
+        <v>352</v>
+      </c>
+      <c r="L131" t="s">
+        <v>13</v>
+      </c>
+      <c r="M131" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>366</v>
+      </c>
+      <c r="B132" t="s">
+        <v>367</v>
+      </c>
+      <c r="C132" t="s">
+        <v>361</v>
+      </c>
+      <c r="D132" t="s">
+        <v>13</v>
+      </c>
+      <c r="E132" t="s">
+        <v>13</v>
+      </c>
+      <c r="F132" t="s">
+        <v>42</v>
+      </c>
+      <c r="G132" t="s">
+        <v>20</v>
+      </c>
+      <c r="H132" t="s">
+        <v>408</v>
+      </c>
+      <c r="I132" t="s">
+        <v>22</v>
+      </c>
+      <c r="J132" t="s">
+        <v>23</v>
+      </c>
+      <c r="K132" t="s">
+        <v>364</v>
+      </c>
+      <c r="L132" t="s">
+        <v>13</v>
+      </c>
+      <c r="M132" t="s">
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>